<commit_message>
added results using PCA
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="60" windowWidth="19092" windowHeight="9516" tabRatio="374" activeTab="3"/>
+    <workbookView xWindow="192" yWindow="60" windowWidth="19092" windowHeight="9516" tabRatio="374" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="lfw" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="144">
   <si>
     <t>[]</t>
   </si>
@@ -429,6 +429,27 @@
   </si>
   <si>
     <t>Desvio Padrão</t>
+  </si>
+  <si>
+    <t>Folder 1 PCA</t>
+  </si>
+  <si>
+    <t>Folder 2 PCA</t>
+  </si>
+  <si>
+    <t>Folder 3 PCA</t>
+  </si>
+  <si>
+    <t>Folder 4 PCA</t>
+  </si>
+  <si>
+    <t>Final PCA</t>
+  </si>
+  <si>
+    <t>Folder  4 PCA</t>
+  </si>
+  <si>
+    <t>Média PCA</t>
   </si>
 </sst>
 </file>
@@ -607,7 +628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -635,16 +656,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -662,6 +673,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -970,11 +996,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="79950976"/>
-        <c:axId val="79952512"/>
+        <c:axId val="172176896"/>
+        <c:axId val="172178432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79950976"/>
+        <c:axId val="172176896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1015,14 +1041,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79952512"/>
+        <c:crossAx val="172178432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79952512"/>
+        <c:axId val="172178432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1072,7 +1098,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79950976"/>
+        <c:crossAx val="172176896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1145,7 +1171,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1471,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R59"/>
+  <dimension ref="A1:AG59"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1482,36 +1508,56 @@
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="E1" s="16" t="s">
+      <c r="C1" s="23"/>
+      <c r="E1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="H1" s="16" t="s">
+      <c r="F1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="K1" s="16" t="s">
+      <c r="I1" s="23"/>
+      <c r="K1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="N1" s="16" t="s">
+      <c r="L1" s="23"/>
+      <c r="N1" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="Q1" s="16" t="s">
+      <c r="O1" s="23"/>
+      <c r="Q1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="16"/>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="R1" s="23"/>
+      <c r="T1" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="U1" s="23"/>
+      <c r="W1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="X1" s="23"/>
+      <c r="Z1" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA1" s="23"/>
+      <c r="AC1" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD1" s="23"/>
+      <c r="AF1" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" s="23"/>
+    </row>
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1551,8 +1597,38 @@
       <c r="R2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1600,8 +1676,40 @@
         <f>AVERAGE(O3:O59)</f>
         <v>0.3849848025549929</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1">
+      <c r="T3">
+        <v>0.5</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0.4</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0.6</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <f>(T3+W3+Z3+AC3)/4</f>
+        <v>0.51388888888888906</v>
+      </c>
+      <c r="AG3">
+        <f>(U3+X3+AA3+AD3)/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="15" thickBot="1">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1641,8 +1749,40 @@
         <f t="shared" ref="O4:O59" si="1">(C4+F4+I4+L4)/4</f>
         <v>0.34027777777777746</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="15.6" thickTop="1" thickBot="1">
+      <c r="T4">
+        <v>0.5</v>
+      </c>
+      <c r="U4">
+        <v>0.5</v>
+      </c>
+      <c r="W4">
+        <v>0.77777777777777801</v>
+      </c>
+      <c r="X4">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="Z4">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="AA4">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="AC4">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="AD4">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" ref="AF4:AF59" si="2">(T4+W4+Z4+AC4)/4</f>
+        <v>0.48611111111111105</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" ref="AG4:AG59" si="3">(U4+X4+AA4+AD4)/4</f>
+        <v>0.23611111111111099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="15.6" thickTop="1" thickBot="1">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1682,12 +1822,44 @@
         <f t="shared" si="1"/>
         <v>0.18333333333333324</v>
       </c>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="R5" s="18"/>
-    </row>
-    <row r="6" spans="1:18" ht="15" thickTop="1">
+      <c r="R5" s="22"/>
+      <c r="T5">
+        <v>0.4</v>
+      </c>
+      <c r="U5">
+        <v>0.2</v>
+      </c>
+      <c r="W5">
+        <v>0.6</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0.2</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="2"/>
+        <v>0.38333333333333325</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="15" thickTop="1">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1727,14 +1899,46 @@
         <f t="shared" si="1"/>
         <v>0.36111111111111099</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="Q6" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="R6" s="20" t="s">
+      <c r="R6" s="16" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="15" thickBot="1">
+      <c r="T6">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="X6">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="Z6">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="AA6">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AC6">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="AD6">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="2"/>
+        <v>0.36111111111111072</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333245E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="15" thickBot="1">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1774,16 +1978,48 @@
         <f t="shared" si="1"/>
         <v>0.66776315789473684</v>
       </c>
-      <c r="Q7" s="21">
-        <f>STDEV(N3:N13)</f>
-        <v>0.27410381111319421</v>
-      </c>
-      <c r="R7" s="22">
-        <f>STDEV(O3:O13)</f>
-        <v>0.24515483320463327</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="15" thickTop="1">
+      <c r="Q7" s="18">
+        <f>STDEV(N3:N59)</f>
+        <v>0.21899944685308567</v>
+      </c>
+      <c r="R7" s="18">
+        <f>STDEV(O3:O59)</f>
+        <v>0.21242534683518519</v>
+      </c>
+      <c r="T7">
+        <v>0.89473684210526305</v>
+      </c>
+      <c r="U7">
+        <v>0.78947368421052599</v>
+      </c>
+      <c r="W7">
+        <v>0.8</v>
+      </c>
+      <c r="X7">
+        <v>0.5</v>
+      </c>
+      <c r="Z7">
+        <v>0.89473684210526305</v>
+      </c>
+      <c r="AA7">
+        <v>0.89473684210526305</v>
+      </c>
+      <c r="AC7">
+        <v>0.7</v>
+      </c>
+      <c r="AD7">
+        <v>0.65</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" si="2"/>
+        <v>0.82236842105263164</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="3"/>
+        <v>0.70855263157894732</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="15" thickTop="1">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1823,8 +2059,40 @@
         <f t="shared" si="1"/>
         <v>0.11818181818181825</v>
       </c>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="T8">
+        <v>0.2</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0.2</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" si="2"/>
+        <v>0.12272727272727273</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1864,8 +2132,44 @@
         <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="Q9" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="R9" s="23"/>
+      <c r="T9">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="U9">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="W9">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="X9">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="Z9">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AD9">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="2"/>
+        <v>0.29166666666666646</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="3"/>
+        <v>0.16666666666666674</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1905,8 +2209,46 @@
         <f t="shared" si="1"/>
         <v>0.28571428571428598</v>
       </c>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="Q10" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="X10">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="Z10">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="2"/>
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="3"/>
+        <v>3.5714285714285747E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1946,8 +2288,48 @@
         <f t="shared" si="1"/>
         <v>0.22500000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="Q11" s="3">
+        <f>AVERAGE(AF3:AF59)</f>
+        <v>0.46963386181231792</v>
+      </c>
+      <c r="R11" s="3">
+        <f>AVERAGE(AG3:AG59)</f>
+        <v>0.20972444146744129</v>
+      </c>
+      <c r="T11">
+        <v>0.8</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0.4</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0.4</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <f t="shared" si="2"/>
+        <v>0.48333333333333328</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" ht="15" thickBot="1">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1987,8 +2369,40 @@
         <f t="shared" si="1"/>
         <v>0.85642655367231624</v>
       </c>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="T12">
+        <v>0.84745762711864403</v>
+      </c>
+      <c r="U12">
+        <v>0.98305084745762705</v>
+      </c>
+      <c r="W12">
+        <v>0.86440677966101698</v>
+      </c>
+      <c r="X12">
+        <v>0.88135593220339004</v>
+      </c>
+      <c r="Z12">
+        <v>0.88135593220339004</v>
+      </c>
+      <c r="AA12">
+        <v>0.96610169491525399</v>
+      </c>
+      <c r="AC12">
+        <v>0.85</v>
+      </c>
+      <c r="AD12">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="2"/>
+        <v>0.86080508474576278</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="3"/>
+        <v>0.93679378531073454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" ht="15.6" thickTop="1" thickBot="1">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2028,8 +2442,44 @@
         <f t="shared" si="1"/>
         <v>3.5714285714285747E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="Q13" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="R13" s="22"/>
+      <c r="T13">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0.25</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0.125</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0.125</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <f t="shared" si="2"/>
+        <v>0.19642857142857151</v>
+      </c>
+      <c r="AG13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" ht="15" thickTop="1">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2069,8 +2519,46 @@
         <f t="shared" si="1"/>
         <v>0.76774193548387071</v>
       </c>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="Q14" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="R14" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="T14">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="U14">
+        <v>0.9</v>
+      </c>
+      <c r="W14">
+        <v>0.8</v>
+      </c>
+      <c r="X14">
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="Z14">
+        <v>0.86666666666666703</v>
+      </c>
+      <c r="AA14">
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="AC14">
+        <v>0.80645161290322598</v>
+      </c>
+      <c r="AD14">
+        <v>0.87096774193548399</v>
+      </c>
+      <c r="AF14">
+        <f t="shared" si="2"/>
+        <v>0.82661290322580649</v>
+      </c>
+      <c r="AG14">
+        <f t="shared" si="3"/>
+        <v>0.80940860215053745</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="15" thickBot="1">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2110,8 +2598,48 @@
         <f t="shared" si="1"/>
         <v>0.22499999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="Q15" s="17">
+        <f>STDEV(AF3:AF59)</f>
+        <v>0.20451803299656779</v>
+      </c>
+      <c r="R15" s="18">
+        <f>STDEV(AG3:AG59)</f>
+        <v>0.24935296164246429</v>
+      </c>
+      <c r="T15">
+        <v>0.4</v>
+      </c>
+      <c r="U15">
+        <v>0.2</v>
+      </c>
+      <c r="W15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0.2</v>
+      </c>
+      <c r="AC15">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <f t="shared" si="2"/>
+        <v>0.35</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="15" thickTop="1">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2151,8 +2679,40 @@
         <f t="shared" si="1"/>
         <v>0.9434666210981999</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="T16">
+        <v>0.88636363636363602</v>
+      </c>
+      <c r="U16">
+        <v>0.96212121212121204</v>
+      </c>
+      <c r="W16">
+        <v>0.86466165413533802</v>
+      </c>
+      <c r="X16">
+        <v>0.96240601503759404</v>
+      </c>
+      <c r="Z16">
+        <v>0.90225563909774398</v>
+      </c>
+      <c r="AA16">
+        <v>0.977443609022556</v>
+      </c>
+      <c r="AC16">
+        <v>0.87969924812030098</v>
+      </c>
+      <c r="AD16">
+        <v>0.98496240601503804</v>
+      </c>
+      <c r="AF16">
+        <f t="shared" si="2"/>
+        <v>0.88324504442925478</v>
+      </c>
+      <c r="AG16">
+        <f t="shared" si="3"/>
+        <v>0.97173331054909995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2192,8 +2752,40 @@
         <f t="shared" si="1"/>
         <v>0.45568783068783075</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="T17">
+        <v>0.592592592592593</v>
+      </c>
+      <c r="U17">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="W17">
+        <v>0.46428571428571402</v>
+      </c>
+      <c r="X17">
+        <v>0.53571428571428603</v>
+      </c>
+      <c r="Z17">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="AA17">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="AC17">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="AD17">
+        <v>0.5</v>
+      </c>
+      <c r="AF17">
+        <f t="shared" si="2"/>
+        <v>0.51025132275132301</v>
+      </c>
+      <c r="AG17">
+        <f t="shared" si="3"/>
+        <v>0.4811507936507935</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2233,8 +2825,40 @@
         <f t="shared" si="1"/>
         <v>0.56818181818181801</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="T18">
+        <v>0.63636363636363602</v>
+      </c>
+      <c r="U18">
+        <v>0.27272727272727298</v>
+      </c>
+      <c r="W18">
+        <v>0.45454545454545497</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0.36363636363636398</v>
+      </c>
+      <c r="AA18">
+        <v>0.18181818181818199</v>
+      </c>
+      <c r="AC18">
+        <v>0.36363636363636398</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <f t="shared" si="2"/>
+        <v>0.45454545454545475</v>
+      </c>
+      <c r="AG18">
+        <f t="shared" si="3"/>
+        <v>0.11363636363636374</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2274,8 +2898,40 @@
         <f t="shared" si="1"/>
         <v>7.1428571428571494E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <f t="shared" si="2"/>
+        <v>7.1428571428571494E-2</v>
+      </c>
+      <c r="AG19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2315,8 +2971,40 @@
         <f t="shared" si="1"/>
         <v>0.52678571428571419</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="T20">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0.875</v>
+      </c>
+      <c r="X20">
+        <v>0.125</v>
+      </c>
+      <c r="Z20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0.625</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <f t="shared" si="2"/>
+        <v>0.76785714285714279</v>
+      </c>
+      <c r="AG20">
+        <f t="shared" si="3"/>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2356,8 +3044,40 @@
         <f t="shared" si="1"/>
         <v>0.14166666666666675</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="T21">
+        <v>0.2</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0.4</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <f t="shared" si="2"/>
+        <v>0.2333333333333335</v>
+      </c>
+      <c r="AG21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2397,8 +3117,40 @@
         <f t="shared" si="1"/>
         <v>0.35833333333333328</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="T22">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="U22">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="W22">
+        <v>0.7</v>
+      </c>
+      <c r="X22">
+        <v>0.4</v>
+      </c>
+      <c r="Z22">
+        <v>0.3</v>
+      </c>
+      <c r="AA22">
+        <v>0.4</v>
+      </c>
+      <c r="AC22">
+        <v>0.3</v>
+      </c>
+      <c r="AD22">
+        <v>0.3</v>
+      </c>
+      <c r="AF22">
+        <f t="shared" si="2"/>
+        <v>0.35277777777777775</v>
+      </c>
+      <c r="AG22">
+        <f t="shared" si="3"/>
+        <v>0.38611111111111102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2438,8 +3190,40 @@
         <f t="shared" si="1"/>
         <v>0.62500000000000033</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="T23">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="X23">
+        <v>0.27777777777777801</v>
+      </c>
+      <c r="Z23">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="AD23">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AF23">
+        <f t="shared" si="2"/>
+        <v>0.61111111111111127</v>
+      </c>
+      <c r="AG23">
+        <f t="shared" si="3"/>
+        <v>9.7222222222222252E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2479,8 +3263,40 @@
         <f t="shared" si="1"/>
         <v>0.57142857142857117</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="T24">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="U24">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="W24">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="X24">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="Z24">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="AA24">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="AC24">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="AD24">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="AF24">
+        <f t="shared" si="2"/>
+        <v>0.46428571428571425</v>
+      </c>
+      <c r="AG24">
+        <f t="shared" si="3"/>
+        <v>0.32142857142857173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2520,8 +3336,40 @@
         <f t="shared" si="1"/>
         <v>0.5657051282051283</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="T25">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="U25">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="W25">
+        <v>0.46153846153846201</v>
+      </c>
+      <c r="X25">
+        <v>0.38461538461538503</v>
+      </c>
+      <c r="Z25">
+        <v>0.61538461538461497</v>
+      </c>
+      <c r="AA25">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="AC25">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="AD25">
+        <v>0.30769230769230799</v>
+      </c>
+      <c r="AF25">
+        <f t="shared" si="2"/>
+        <v>0.5657051282051283</v>
+      </c>
+      <c r="AG25">
+        <f t="shared" si="3"/>
+        <v>0.41185897435897445</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2561,8 +3409,40 @@
         <f t="shared" si="1"/>
         <v>0.54532967032967017</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="T26">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="U26">
+        <v>0.230769230769231</v>
+      </c>
+      <c r="W26">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="X26">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="Z26">
+        <v>0.64285714285714302</v>
+      </c>
+      <c r="AA26">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="AC26">
+        <v>0.64285714285714302</v>
+      </c>
+      <c r="AD26">
+        <v>0.35714285714285698</v>
+      </c>
+      <c r="AF26">
+        <f t="shared" si="2"/>
+        <v>0.59890109890109877</v>
+      </c>
+      <c r="AG26">
+        <f t="shared" si="3"/>
+        <v>0.32554945054945073</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2602,8 +3482,40 @@
         <f t="shared" si="1"/>
         <v>0.18333333333333324</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="T27">
+        <v>0.8</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0.8</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0.8</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>0.5</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <f t="shared" si="2"/>
+        <v>0.72500000000000009</v>
+      </c>
+      <c r="AG27">
+        <f>(U27+X27+AA27+AD27)/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2643,8 +3555,40 @@
         <f t="shared" si="1"/>
         <v>0.59999999999999976</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="T28">
+        <v>0.4</v>
+      </c>
+      <c r="U28">
+        <v>0.2</v>
+      </c>
+      <c r="W28">
+        <v>0.45454545454545497</v>
+      </c>
+      <c r="X28">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="Z28">
+        <v>0.45454545454545497</v>
+      </c>
+      <c r="AA28">
+        <v>0.27272727272727298</v>
+      </c>
+      <c r="AC28">
+        <v>0.45454545454545497</v>
+      </c>
+      <c r="AD28">
+        <v>0.18181818181818199</v>
+      </c>
+      <c r="AF28">
+        <f t="shared" si="2"/>
+        <v>0.44090909090909125</v>
+      </c>
+      <c r="AG28">
+        <f t="shared" si="3"/>
+        <v>0.18636363636363648</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2684,8 +3628,40 @@
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="T29">
+        <v>0.2</v>
+      </c>
+      <c r="U29">
+        <v>0.2</v>
+      </c>
+      <c r="W29">
+        <v>0.8</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>1</v>
+      </c>
+      <c r="AA29">
+        <v>0.2</v>
+      </c>
+      <c r="AC29">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AD29">
+        <v>0</v>
+      </c>
+      <c r="AF29">
+        <f t="shared" si="2"/>
+        <v>0.54166666666666674</v>
+      </c>
+      <c r="AG29">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2725,8 +3701,40 @@
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="T30">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="U30">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="W30">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="X30">
+        <v>0.5</v>
+      </c>
+      <c r="Z30">
+        <v>0.5</v>
+      </c>
+      <c r="AA30">
+        <v>0</v>
+      </c>
+      <c r="AC30">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="AD30">
+        <v>0</v>
+      </c>
+      <c r="AF30">
+        <f t="shared" si="2"/>
+        <v>0.39880952380952378</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="3"/>
+        <v>0.16666666666666674</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2766,8 +3774,40 @@
         <f t="shared" si="1"/>
         <v>0.34478021978021972</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="T31">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="U31">
+        <v>0.15384615384615399</v>
+      </c>
+      <c r="W31">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="X31">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="Z31">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="AA31">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="AC31">
+        <v>0.64285714285714302</v>
+      </c>
+      <c r="AD31">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="AF31">
+        <f t="shared" si="2"/>
+        <v>0.45604395604395587</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="3"/>
+        <v>0.28846153846153849</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2807,8 +3847,40 @@
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="T32">
+        <v>0.125</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0.25</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <v>0.25</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AC32">
+        <v>0.25</v>
+      </c>
+      <c r="AD32">
+        <v>0</v>
+      </c>
+      <c r="AF32">
+        <f t="shared" si="2"/>
+        <v>0.21875</v>
+      </c>
+      <c r="AG32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2848,8 +3920,40 @@
         <f>(C33+F33+I33+L33)/4</f>
         <v>0.34166666666666651</v>
       </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="T33">
+        <v>0.2</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="X33">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="Z33">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AA33">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AC33">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AD33">
+        <v>0</v>
+      </c>
+      <c r="AF33">
+        <f t="shared" si="2"/>
+        <v>0.21666666666666673</v>
+      </c>
+      <c r="AG33">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333495E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2889,8 +3993,40 @@
         <f t="shared" si="1"/>
         <v>0.17857142857142874</v>
       </c>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="T34">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="U34">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="W34">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="AA34">
+        <v>0</v>
+      </c>
+      <c r="AC34">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="AD34">
+        <v>0</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" si="2"/>
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="3"/>
+        <v>3.5714285714285747E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2930,8 +4066,40 @@
         <f t="shared" si="1"/>
         <v>0.67738095238095242</v>
       </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="T35">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="U35">
+        <v>0.35714285714285698</v>
+      </c>
+      <c r="W35">
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="X35">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="Z35">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="AA35">
+        <v>0.8</v>
+      </c>
+      <c r="AC35">
+        <v>0.86666666666666703</v>
+      </c>
+      <c r="AD35">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="AF35">
+        <f t="shared" si="2"/>
+        <v>0.70952380952380945</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" si="3"/>
+        <v>0.55595238095238075</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2971,8 +4139,40 @@
         <f t="shared" si="1"/>
         <v>0.45833333333333326</v>
       </c>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="T36">
+        <v>0.625</v>
+      </c>
+      <c r="U36">
+        <v>0.375</v>
+      </c>
+      <c r="W36">
+        <v>0.75</v>
+      </c>
+      <c r="X36">
+        <v>0.375</v>
+      </c>
+      <c r="Z36">
+        <v>0.375</v>
+      </c>
+      <c r="AA36">
+        <v>0</v>
+      </c>
+      <c r="AC36">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="AD36">
+        <v>0</v>
+      </c>
+      <c r="AF36">
+        <f t="shared" si="2"/>
+        <v>0.60416666666666674</v>
+      </c>
+      <c r="AG36">
+        <f t="shared" si="3"/>
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -3012,8 +4212,40 @@
         <f t="shared" si="1"/>
         <v>0.6068181818181817</v>
       </c>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="T37">
+        <v>0.4</v>
+      </c>
+      <c r="U37">
+        <v>0.3</v>
+      </c>
+      <c r="W37">
+        <v>0.8</v>
+      </c>
+      <c r="X37">
+        <v>0.4</v>
+      </c>
+      <c r="Z37">
+        <v>0.8</v>
+      </c>
+      <c r="AA37">
+        <v>0</v>
+      </c>
+      <c r="AC37">
+        <v>0.63636363636363602</v>
+      </c>
+      <c r="AD37">
+        <v>0</v>
+      </c>
+      <c r="AF37">
+        <f t="shared" si="2"/>
+        <v>0.65909090909090895</v>
+      </c>
+      <c r="AG37">
+        <f t="shared" si="3"/>
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -3053,8 +4285,40 @@
         <f t="shared" si="1"/>
         <v>0.31666666666666676</v>
       </c>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="T38">
+        <v>0.4</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>0.5</v>
+      </c>
+      <c r="X38">
+        <v>0</v>
+      </c>
+      <c r="Z38">
+        <v>0.6</v>
+      </c>
+      <c r="AA38">
+        <v>0</v>
+      </c>
+      <c r="AC38">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AD38">
+        <v>0</v>
+      </c>
+      <c r="AF38">
+        <f t="shared" si="2"/>
+        <v>0.41666666666666674</v>
+      </c>
+      <c r="AG38">
+        <f>(U38+X38+AA38+AD38)/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -3094,8 +4358,40 @@
         <f t="shared" si="1"/>
         <v>0.43636363636363623</v>
       </c>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="T39">
+        <v>0.4</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0.6</v>
+      </c>
+      <c r="X39">
+        <v>0.1</v>
+      </c>
+      <c r="Z39">
+        <v>0.6</v>
+      </c>
+      <c r="AA39">
+        <v>0.1</v>
+      </c>
+      <c r="AC39">
+        <v>0.63636363636363602</v>
+      </c>
+      <c r="AD39">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="AF39">
+        <f t="shared" si="2"/>
+        <v>0.55909090909090908</v>
+      </c>
+      <c r="AG39">
+        <f t="shared" si="3"/>
+        <v>7.2727272727272724E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -3135,8 +4431,40 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="T40">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="U40">
+        <v>0.5</v>
+      </c>
+      <c r="W40">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="X40">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="Z40">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="AA40">
+        <v>0.5</v>
+      </c>
+      <c r="AC40">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="AD40">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="AF40">
+        <f t="shared" si="2"/>
+        <v>0.77083333333333348</v>
+      </c>
+      <c r="AG40">
+        <f t="shared" si="3"/>
+        <v>0.58333333333333348</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -3176,8 +4504,40 @@
         <f t="shared" si="1"/>
         <v>0.20982142857142849</v>
       </c>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="T41">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="X41">
+        <v>0</v>
+      </c>
+      <c r="Z41">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="AA41">
+        <v>0</v>
+      </c>
+      <c r="AC41">
+        <v>0.5</v>
+      </c>
+      <c r="AD41">
+        <v>0</v>
+      </c>
+      <c r="AF41">
+        <f t="shared" si="2"/>
+        <v>0.51785714285714302</v>
+      </c>
+      <c r="AG41">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -3217,8 +4577,40 @@
         <f t="shared" si="1"/>
         <v>0.63541666666666674</v>
       </c>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="T42">
+        <v>0.75</v>
+      </c>
+      <c r="U42">
+        <v>0.125</v>
+      </c>
+      <c r="W42">
+        <v>0.5</v>
+      </c>
+      <c r="X42">
+        <v>0</v>
+      </c>
+      <c r="Z42">
+        <v>0.75</v>
+      </c>
+      <c r="AA42">
+        <v>0.125</v>
+      </c>
+      <c r="AC42">
+        <v>0.77777777777777801</v>
+      </c>
+      <c r="AD42">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="AF42">
+        <f t="shared" si="2"/>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="AG42">
+        <f t="shared" si="3"/>
+        <v>0.1180555555555555</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -3258,8 +4650,40 @@
         <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
       </c>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="T43">
+        <v>0.4</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="W43">
+        <v>0.2</v>
+      </c>
+      <c r="X43">
+        <v>0</v>
+      </c>
+      <c r="Z43">
+        <v>0.4</v>
+      </c>
+      <c r="AA43">
+        <v>0</v>
+      </c>
+      <c r="AC43">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AD43">
+        <v>0</v>
+      </c>
+      <c r="AF43">
+        <f>(T43+W43+Z43+AC43)/4</f>
+        <v>0.29166666666666674</v>
+      </c>
+      <c r="AG43">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -3299,8 +4723,40 @@
         <f t="shared" si="1"/>
         <v>0.27500000000000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="T44">
+        <v>0.4</v>
+      </c>
+      <c r="U44">
+        <v>0.3</v>
+      </c>
+      <c r="W44">
+        <v>0.4</v>
+      </c>
+      <c r="X44">
+        <v>0.4</v>
+      </c>
+      <c r="Z44">
+        <v>0.5</v>
+      </c>
+      <c r="AA44">
+        <v>0.1</v>
+      </c>
+      <c r="AC44">
+        <v>0.2</v>
+      </c>
+      <c r="AD44">
+        <v>0.1</v>
+      </c>
+      <c r="AF44">
+        <f t="shared" si="2"/>
+        <v>0.375</v>
+      </c>
+      <c r="AG44">
+        <f t="shared" si="3"/>
+        <v>0.22499999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -3340,8 +4796,40 @@
         <f t="shared" si="1"/>
         <v>0.23333333333333325</v>
       </c>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="T45">
+        <v>0.2</v>
+      </c>
+      <c r="U45">
+        <v>0</v>
+      </c>
+      <c r="W45">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="X45">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="Z45">
+        <v>0</v>
+      </c>
+      <c r="AA45">
+        <v>0.2</v>
+      </c>
+      <c r="AC45">
+        <v>0</v>
+      </c>
+      <c r="AD45">
+        <v>0</v>
+      </c>
+      <c r="AF45">
+        <f t="shared" si="2"/>
+        <v>9.1666666666666757E-2</v>
+      </c>
+      <c r="AG45">
+        <f t="shared" si="3"/>
+        <v>9.1666666666666757E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -3381,8 +4869,40 @@
         <f t="shared" si="1"/>
         <v>0.35267857142857151</v>
       </c>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="T46">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <v>0.5</v>
+      </c>
+      <c r="X46">
+        <v>0</v>
+      </c>
+      <c r="Z46">
+        <v>0.375</v>
+      </c>
+      <c r="AA46">
+        <v>0</v>
+      </c>
+      <c r="AC46">
+        <v>0.625</v>
+      </c>
+      <c r="AD46">
+        <v>0</v>
+      </c>
+      <c r="AF46">
+        <f t="shared" si="2"/>
+        <v>0.48214285714285726</v>
+      </c>
+      <c r="AG46">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -3422,8 +4942,40 @@
         <f t="shared" si="1"/>
         <v>0.25595238095238126</v>
       </c>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="T47">
+        <v>0.5</v>
+      </c>
+      <c r="U47">
+        <v>0</v>
+      </c>
+      <c r="W47">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="X47">
+        <v>0</v>
+      </c>
+      <c r="Z47">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="AA47">
+        <v>0</v>
+      </c>
+      <c r="AC47">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="AD47">
+        <v>0</v>
+      </c>
+      <c r="AF47">
+        <f t="shared" si="2"/>
+        <v>0.51785714285714279</v>
+      </c>
+      <c r="AG47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -3463,8 +5015,40 @@
         <f t="shared" si="1"/>
         <v>0.46875</v>
       </c>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="T48">
+        <v>0.75</v>
+      </c>
+      <c r="U48">
+        <v>0.25</v>
+      </c>
+      <c r="W48">
+        <v>0.875</v>
+      </c>
+      <c r="X48">
+        <v>0</v>
+      </c>
+      <c r="Z48">
+        <v>0.875</v>
+      </c>
+      <c r="AA48">
+        <v>0</v>
+      </c>
+      <c r="AC48">
+        <v>0.875</v>
+      </c>
+      <c r="AD48">
+        <v>0.125</v>
+      </c>
+      <c r="AF48">
+        <f t="shared" si="2"/>
+        <v>0.84375</v>
+      </c>
+      <c r="AG48">
+        <f t="shared" si="3"/>
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -3504,8 +5088,40 @@
         <f t="shared" si="1"/>
         <v>0.16071428571428575</v>
       </c>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="T49">
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="X49">
+        <v>0</v>
+      </c>
+      <c r="Z49">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AA49">
+        <v>0</v>
+      </c>
+      <c r="AC49">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="AD49">
+        <v>0</v>
+      </c>
+      <c r="AF49">
+        <f t="shared" si="2"/>
+        <v>0.22023809523809551</v>
+      </c>
+      <c r="AG49">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -3545,8 +5161,40 @@
         <f t="shared" si="1"/>
         <v>0.61666666666666647</v>
       </c>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="T50">
+        <v>0.8</v>
+      </c>
+      <c r="U50">
+        <v>0.4</v>
+      </c>
+      <c r="W50">
+        <v>0.5</v>
+      </c>
+      <c r="X50">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="Z50">
+        <v>0.5</v>
+      </c>
+      <c r="AA50">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="AC50">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AD50">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="AF50">
+        <f t="shared" si="2"/>
+        <v>0.49166666666666675</v>
+      </c>
+      <c r="AG50">
+        <f>(U50+X50+AA50+AD50)/4</f>
+        <v>0.43333333333333324</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -3586,8 +5234,40 @@
         <f t="shared" si="1"/>
         <v>0.63461538461538425</v>
       </c>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="T51">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="U51">
+        <v>0.30769230769230799</v>
+      </c>
+      <c r="W51">
+        <v>0.46153846153846201</v>
+      </c>
+      <c r="X51">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="Z51">
+        <v>0.15384615384615399</v>
+      </c>
+      <c r="AA51">
+        <v>0.30769230769230799</v>
+      </c>
+      <c r="AC51">
+        <v>0.46153846153846201</v>
+      </c>
+      <c r="AD51">
+        <v>0.230769230769231</v>
+      </c>
+      <c r="AF51">
+        <f t="shared" si="2"/>
+        <v>0.40384615384615397</v>
+      </c>
+      <c r="AG51">
+        <f t="shared" si="3"/>
+        <v>0.34615384615384626</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -3627,8 +5307,40 @@
         <f t="shared" si="1"/>
         <v>0.2430555555555555</v>
       </c>
-    </row>
-    <row r="53" spans="1:15">
+      <c r="T52">
+        <v>0.5</v>
+      </c>
+      <c r="U52">
+        <v>0.125</v>
+      </c>
+      <c r="W52">
+        <v>0.125</v>
+      </c>
+      <c r="X52">
+        <v>0.25</v>
+      </c>
+      <c r="Z52">
+        <v>0.125</v>
+      </c>
+      <c r="AA52">
+        <v>0.5</v>
+      </c>
+      <c r="AC52">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="AD52">
+        <v>0</v>
+      </c>
+      <c r="AF52">
+        <f t="shared" si="2"/>
+        <v>0.32638888888888901</v>
+      </c>
+      <c r="AG52">
+        <f t="shared" si="3"/>
+        <v>0.21875</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -3668,8 +5380,40 @@
         <f t="shared" si="1"/>
         <v>0.16666666666666674</v>
       </c>
-    </row>
-    <row r="54" spans="1:15">
+      <c r="T53">
+        <v>0</v>
+      </c>
+      <c r="U53">
+        <v>0</v>
+      </c>
+      <c r="W53">
+        <v>0.5</v>
+      </c>
+      <c r="X53">
+        <v>0</v>
+      </c>
+      <c r="Z53">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AA53">
+        <v>0.5</v>
+      </c>
+      <c r="AC53">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="AD53">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AF53">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="AG53">
+        <f t="shared" si="3"/>
+        <v>0.16666666666666674</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -3709,8 +5453,40 @@
         <f t="shared" si="1"/>
         <v>8.3333333333333495E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:15">
+      <c r="T54">
+        <v>0.5</v>
+      </c>
+      <c r="U54">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="W54">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="X54">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="Z54">
+        <v>0.5</v>
+      </c>
+      <c r="AA54">
+        <v>0</v>
+      </c>
+      <c r="AC54">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="AD54">
+        <v>0</v>
+      </c>
+      <c r="AF54">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="AG54">
+        <f t="shared" si="3"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -3750,8 +5526,40 @@
         <f t="shared" si="1"/>
         <v>0.23958333333333326</v>
       </c>
-    </row>
-    <row r="56" spans="1:15">
+      <c r="T55">
+        <v>0.5</v>
+      </c>
+      <c r="U55">
+        <v>0</v>
+      </c>
+      <c r="W55">
+        <v>0.5</v>
+      </c>
+      <c r="X55">
+        <v>0.125</v>
+      </c>
+      <c r="Z55">
+        <v>0</v>
+      </c>
+      <c r="AA55">
+        <v>0</v>
+      </c>
+      <c r="AC55">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="AD55">
+        <v>0</v>
+      </c>
+      <c r="AF55">
+        <f t="shared" si="2"/>
+        <v>0.36111111111111099</v>
+      </c>
+      <c r="AG55">
+        <f t="shared" si="3"/>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -3791,8 +5599,40 @@
         <f t="shared" si="1"/>
         <v>0.72222222222222232</v>
       </c>
-    </row>
-    <row r="57" spans="1:15">
+      <c r="T56">
+        <v>0.77777777777777801</v>
+      </c>
+      <c r="U56">
+        <v>0.75</v>
+      </c>
+      <c r="W56">
+        <v>0.5</v>
+      </c>
+      <c r="X56">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="Z56">
+        <v>0.5</v>
+      </c>
+      <c r="AA56">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="AC56">
+        <v>0.75</v>
+      </c>
+      <c r="AD56">
+        <v>0.75</v>
+      </c>
+      <c r="AF56">
+        <f t="shared" si="2"/>
+        <v>0.63194444444444453</v>
+      </c>
+      <c r="AG56">
+        <f t="shared" si="3"/>
+        <v>0.74305555555555547</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -3832,8 +5672,40 @@
         <f t="shared" si="1"/>
         <v>0.28125</v>
       </c>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="T57">
+        <v>0.125</v>
+      </c>
+      <c r="U57">
+        <v>0.125</v>
+      </c>
+      <c r="W57">
+        <v>0.625</v>
+      </c>
+      <c r="X57">
+        <v>0.25</v>
+      </c>
+      <c r="Z57">
+        <v>0.125</v>
+      </c>
+      <c r="AA57">
+        <v>0</v>
+      </c>
+      <c r="AC57">
+        <v>0.25</v>
+      </c>
+      <c r="AD57">
+        <v>0</v>
+      </c>
+      <c r="AF57">
+        <f t="shared" si="2"/>
+        <v>0.28125</v>
+      </c>
+      <c r="AG57">
+        <f t="shared" si="3"/>
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:33">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -3873,8 +5745,40 @@
         <f t="shared" si="1"/>
         <v>0.34090909090909099</v>
       </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="T58">
+        <v>0.27272727272727298</v>
+      </c>
+      <c r="U58">
+        <v>0.18181818181818199</v>
+      </c>
+      <c r="W58">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="X58">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="Z58">
+        <v>0.25</v>
+      </c>
+      <c r="AA58">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AC58">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="AD58">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="AF58">
+        <f t="shared" si="2"/>
+        <v>0.33901515151515177</v>
+      </c>
+      <c r="AG58">
+        <f t="shared" si="3"/>
+        <v>0.14962121212121229</v>
+      </c>
+    </row>
+    <row r="59" spans="1:33">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -3914,9 +5818,48 @@
         <f t="shared" si="1"/>
         <v>0.45833333333333326</v>
       </c>
+      <c r="T59">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="U59">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="W59">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="X59">
+        <v>0.5</v>
+      </c>
+      <c r="Z59">
+        <v>0.5</v>
+      </c>
+      <c r="AA59">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="AC59">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="AD59">
+        <v>0.5</v>
+      </c>
+      <c r="AF59">
+        <f t="shared" si="2"/>
+        <v>0.54166666666666674</v>
+      </c>
+      <c r="AG59">
+        <f t="shared" si="3"/>
+        <v>0.41666666666666652</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AF1:AG1"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="E1:F1"/>
@@ -3941,30 +5884,30 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="E1" s="16" t="s">
+      <c r="C1" s="23"/>
+      <c r="E1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="H1" s="16" t="s">
+      <c r="F1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="K1" s="16" t="s">
+      <c r="I1" s="23"/>
+      <c r="K1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="N1" s="16" t="s">
+      <c r="L1" s="23"/>
+      <c r="N1" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="Q1" s="16" t="s">
+      <c r="O1" s="23"/>
+      <c r="Q1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="16"/>
+      <c r="R1" s="23"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
@@ -4137,10 +6080,10 @@
         <f t="shared" si="1"/>
         <v>0.70833333333333326</v>
       </c>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="R5" s="18"/>
+      <c r="R5" s="22"/>
     </row>
     <row r="6" spans="1:18" ht="15" thickTop="1">
       <c r="A6" t="s">
@@ -4182,10 +6125,10 @@
         <f t="shared" si="1"/>
         <v>0.83333333333333326</v>
       </c>
-      <c r="Q6" s="23" t="s">
+      <c r="Q6" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="R6" s="24" t="s">
+      <c r="R6" s="20" t="s">
         <v>120</v>
       </c>
     </row>
@@ -4229,11 +6172,11 @@
         <f t="shared" si="1"/>
         <v>0.91666666666666674</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="17">
         <f>STDEV(N3:N13)</f>
         <v>8.4274982807905255E-2</v>
       </c>
-      <c r="R7" s="22">
+      <c r="R7" s="18">
         <f>STDEV(O3:O13)</f>
         <v>0.12398578445722946</v>
       </c>
@@ -5690,39 +7633,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="E1" s="16" t="s">
+      <c r="C1" s="23"/>
+      <c r="E1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="H1" s="16" t="s">
+      <c r="F1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="K1" s="16" t="s">
+      <c r="I1" s="23"/>
+      <c r="K1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="N1" s="16" t="s">
+      <c r="L1" s="23"/>
+      <c r="N1" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="Q1" s="16" t="s">
+      <c r="O1" s="23"/>
+      <c r="Q1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="16"/>
+      <c r="R1" s="23"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
@@ -5904,10 +7847,10 @@
         <v>0.83653846153846145</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="R5" s="18"/>
+      <c r="R5" s="22"/>
     </row>
     <row r="6" spans="1:18" ht="15" thickTop="1">
       <c r="A6" t="s">
@@ -5950,10 +7893,10 @@
         <v>0.80769230769230749</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="19" t="s">
+      <c r="Q6" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="R6" s="20" t="s">
+      <c r="R6" s="16" t="s">
         <v>120</v>
       </c>
     </row>
@@ -5998,11 +7941,11 @@
         <v>0.79166666666666674</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="21">
+      <c r="Q7" s="17">
         <f>STDEV(N3:N13)</f>
         <v>8.8036409152898967E-2</v>
       </c>
-      <c r="R7" s="22">
+      <c r="R7" s="18">
         <f>STDEV(O3:O13)</f>
         <v>0.10596897838923086</v>
       </c>
@@ -6272,10 +8215,511 @@
       <c r="R13" s="3"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="B15" s="15"/>
+      <c r="B15" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="E15" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="H15" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="I15" s="23"/>
+      <c r="K15" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="L15" s="23"/>
+      <c r="N15" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="O15" s="23"/>
+      <c r="Q15" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="R15" s="23"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="25">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="C17" s="25">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0.75</v>
+      </c>
+      <c r="F17">
+        <v>0.875</v>
+      </c>
+      <c r="H17">
+        <v>0.875</v>
+      </c>
+      <c r="I17">
+        <v>0.75</v>
+      </c>
+      <c r="K17">
+        <v>0.375</v>
+      </c>
+      <c r="L17">
+        <v>0.75</v>
+      </c>
+      <c r="N17">
+        <f>(B17+E17+H17+K17)/4</f>
+        <v>0.71428571428571419</v>
+      </c>
+      <c r="O17">
+        <f>(C17+F17+I17+L17)/4</f>
+        <v>0.84375</v>
+      </c>
+      <c r="Q17" s="3">
+        <f>AVERAGE(N17:N27)</f>
+        <v>0.84131663790754696</v>
+      </c>
+      <c r="R17" s="3">
+        <f>AVERAGE(O17:O27)</f>
+        <v>0.86274615535979171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15" thickBot="1">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="25">
+        <v>1</v>
+      </c>
+      <c r="C18" s="25">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0.90909090909090895</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0.81818181818181801</v>
+      </c>
+      <c r="L18">
+        <v>0.90909090909090895</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ref="N18:N27" si="2">(B18+E18+H18+K18)/4</f>
+        <v>0.93181818181818177</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18:O27" si="3">(C18+F18+I18+L18)/4</f>
+        <v>0.97727272727272729</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="25">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="C19" s="25">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="L19">
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>0.92147435897435903</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="3"/>
+        <v>0.93910256410256399</v>
+      </c>
+      <c r="Q19" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="R19" s="22"/>
+    </row>
+    <row r="20" spans="1:18" ht="15" thickTop="1">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="25">
+        <v>0.84615384615384603</v>
+      </c>
+      <c r="C20" s="25">
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="E20">
+        <v>0.61538461538461497</v>
+      </c>
+      <c r="F20">
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="H20">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="I20">
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="K20">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="L20">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="3"/>
+        <v>0.88461538461538458</v>
+      </c>
+      <c r="Q20" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="R20" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15" thickBot="1">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="25">
+        <v>1</v>
+      </c>
+      <c r="C21" s="25">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="F21">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="H21">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="I21">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="K21">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="L21">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="2"/>
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="3"/>
+        <v>0.87499999999999978</v>
+      </c>
+      <c r="Q21" s="17">
+        <f>STDEV(N17:N27)</f>
+        <v>0.10077059844082589</v>
+      </c>
+      <c r="R21" s="18">
+        <f>STDEV(O17:O27)</f>
+        <v>9.6271202356662464E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15" thickTop="1">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="25">
+        <v>0.69230769230769196</v>
+      </c>
+      <c r="C22" s="25">
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="E22">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="F22">
+        <v>0.61538461538461497</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0.84615384615384603</v>
+      </c>
+      <c r="L22">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="2"/>
+        <v>0.82692307692307665</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="3"/>
+        <v>0.82692307692307676</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="25">
+        <v>0.84615384615384603</v>
+      </c>
+      <c r="C23" s="25">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0.84615384615384603</v>
+      </c>
+      <c r="F23">
+        <v>0.84615384615384603</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="2"/>
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="3"/>
+        <v>0.88461538461538458</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="C24" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0.8</v>
+      </c>
+      <c r="I24">
+        <v>0.6</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>0.6</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="3"/>
+        <v>0.92857142857142838</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="25">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="C26" s="25">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>0.91666666666666652</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="3"/>
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="25">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="C27" s="25">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="I27">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="K27">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="L27">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="2"/>
+        <v>0.72023809523809501</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="3"/>
+        <v>0.64285714285714279</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="N15:O15"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="B1:C1"/>
@@ -6293,7 +8737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
@@ -6308,30 +8752,30 @@
       <c r="A1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="E1" s="16" t="s">
+      <c r="C1" s="23"/>
+      <c r="E1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="H1" s="16" t="s">
+      <c r="F1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="K1" s="16" t="s">
+      <c r="I1" s="23"/>
+      <c r="K1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="N1" s="16" t="s">
+      <c r="L1" s="23"/>
+      <c r="N1" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="Q1" s="16" t="s">
+      <c r="O1" s="23"/>
+      <c r="Q1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="16"/>
+      <c r="R1" s="23"/>
     </row>
     <row r="2" spans="1:18">
       <c r="B2" t="s">
@@ -6506,10 +8950,10 @@
         <v>1</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="R5" s="18"/>
+      <c r="R5" s="22"/>
     </row>
     <row r="6" spans="1:18" ht="15" thickTop="1">
       <c r="A6" s="2" t="s">
@@ -6552,10 +8996,10 @@
         <v>1</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="19" t="s">
+      <c r="Q6" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="R6" s="20" t="s">
+      <c r="R6" s="16" t="s">
         <v>120</v>
       </c>
     </row>
@@ -6600,11 +9044,11 @@
         <v>1</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="21">
+      <c r="Q7" s="17">
         <f>STDEV(N3:N13)</f>
         <v>2.7718773065873566E-2</v>
       </c>
-      <c r="R7" s="22">
+      <c r="R7" s="18">
         <f>STDEV(O3:O13)</f>
         <v>2.6352313834736473E-2</v>
       </c>

</xml_diff>